<commit_message>
restructure input and output folder
</commit_message>
<xml_diff>
--- a/IRQ_2021HNO_Inter-sectoral_PIN-Severity_DRAFT-ENDORSED_AWG-IMWG_2020_09_03.xlsx
+++ b/IRQ_2021HNO_Inter-sectoral_PIN-Severity_DRAFT-ENDORSED_AWG-IMWG_2020_09_03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\OneDrive\Documents\REACH2020\MCNA VIII\6. Data Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\OneDrive\Documents\REACH2020\MCNA VIII\MCNA20_Analysis_IRQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475A7CF4-C937-4C27-9805-2CBCB9E29A4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F244538-4739-4513-AFD7-CEAE341313B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DE93082-DA25-4047-BA9C-ECE0BEA4BEF8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DE93082-DA25-4047-BA9C-ECE0BEA4BEF8}"/>
   </bookViews>
   <sheets>
     <sheet name="IRQ2021_Intercluster_PIN_Sev" sheetId="1" r:id="rId1"/>
@@ -2243,6 +2243,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2255,61 +2273,43 @@
     <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2770,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2565E548-5449-442A-A965-6E689A09088F}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="83" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2863,22 +2863,22 @@
     <row r="5" spans="1:15" s="76" customFormat="1" ht="34.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="72"/>
       <c r="B5" s="73"/>
-      <c r="C5" s="141" t="s">
+      <c r="C5" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="142"/>
+      <c r="D5" s="148"/>
       <c r="E5" s="77" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="74"/>
       <c r="G5" s="74"/>
-      <c r="H5" s="143" t="s">
+      <c r="H5" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
-      <c r="K5" s="144"/>
-      <c r="L5" s="144"/>
+      <c r="I5" s="150"/>
+      <c r="J5" s="150"/>
+      <c r="K5" s="150"/>
+      <c r="L5" s="150"/>
       <c r="M5" s="82"/>
       <c r="N5" s="75"/>
       <c r="O5" s="79" t="s">
@@ -2904,7 +2904,7 @@
       <c r="F6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="158" t="s">
+      <c r="G6" s="141" t="s">
         <v>207</v>
       </c>
       <c r="H6" s="17" t="s">
@@ -3160,18 +3160,16 @@
       <c r="D12" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="161" t="s">
+      <c r="E12" s="144" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="160" t="s">
+      <c r="F12" s="143" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="160" t="s">
+      <c r="G12" s="143" t="s">
         <v>212</v>
       </c>
-      <c r="H12" s="161" t="s">
-        <v>25</v>
-      </c>
+      <c r="H12" s="144"/>
       <c r="I12" s="98" t="s">
         <v>57</v>
       </c>
@@ -3257,7 +3255,9 @@
       <c r="G14" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="H14" s="44"/>
+      <c r="H14" s="44" t="s">
+        <v>25</v>
+      </c>
       <c r="I14" s="98" t="s">
         <v>71</v>
       </c>
@@ -3590,13 +3590,13 @@
       <c r="D22" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="162" t="s">
+      <c r="E22" s="145" t="s">
         <v>118</v>
       </c>
-      <c r="F22" s="163" t="s">
+      <c r="F22" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="163" t="s">
+      <c r="G22" s="146" t="s">
         <v>226</v>
       </c>
       <c r="H22" s="39"/>
@@ -3768,7 +3768,7 @@
       <c r="F26" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="159" t="s">
+      <c r="G26" s="142" t="s">
         <v>223</v>
       </c>
       <c r="H26" s="62" t="s">
@@ -3967,367 +3967,341 @@
       <c r="B3" s="138" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="155" t="s">
+      <c r="C3" s="151" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="155"/>
-      <c r="E3" s="155"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
-      <c r="K3" s="155"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
       <c r="L3" s="138" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="156">
+      <c r="A4" s="152">
         <v>1</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="152" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="153" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
-      <c r="F4" s="157"/>
-      <c r="G4" s="157"/>
-      <c r="H4" s="157"/>
-      <c r="I4" s="157"/>
-      <c r="J4" s="157"/>
-      <c r="K4" s="157"/>
-      <c r="L4" s="157" t="s">
+      <c r="D4" s="153"/>
+      <c r="E4" s="153"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="153"/>
+      <c r="K4" s="153"/>
+      <c r="L4" s="153" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="156"/>
-      <c r="B5" s="156"/>
-      <c r="C5" s="157" t="s">
+      <c r="A5" s="152"/>
+      <c r="B5" s="152"/>
+      <c r="C5" s="153" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
-      <c r="G5" s="157"/>
-      <c r="H5" s="157"/>
-      <c r="I5" s="157"/>
-      <c r="J5" s="157"/>
-      <c r="K5" s="157"/>
-      <c r="L5" s="157"/>
+      <c r="D5" s="153"/>
+      <c r="E5" s="153"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
+      <c r="K5" s="153"/>
+      <c r="L5" s="153"/>
     </row>
     <row r="6" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="156"/>
-      <c r="B6" s="156"/>
-      <c r="C6" s="157" t="s">
+      <c r="A6" s="152"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="153" t="s">
         <v>173</v>
       </c>
-      <c r="D6" s="157"/>
-      <c r="E6" s="157"/>
-      <c r="F6" s="157"/>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="157"/>
-      <c r="K6" s="157"/>
-      <c r="L6" s="157"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="153"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="153"/>
     </row>
     <row r="7" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="153">
+      <c r="A7" s="154">
         <v>2</v>
       </c>
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="154" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="154" t="s">
+      <c r="C7" s="155" t="s">
         <v>175</v>
       </c>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="154"/>
-      <c r="G7" s="154"/>
-      <c r="H7" s="154"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="154"/>
-      <c r="K7" s="154"/>
-      <c r="L7" s="154" t="s">
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="155"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="155"/>
+      <c r="J7" s="155"/>
+      <c r="K7" s="155"/>
+      <c r="L7" s="155" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="153"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="154" t="s">
+      <c r="A8" s="154"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="155" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="154"/>
-      <c r="G8" s="154"/>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
-      <c r="K8" s="154"/>
-      <c r="L8" s="154"/>
+      <c r="D8" s="155"/>
+      <c r="E8" s="155"/>
+      <c r="F8" s="155"/>
+      <c r="G8" s="155"/>
+      <c r="H8" s="155"/>
+      <c r="I8" s="155"/>
+      <c r="J8" s="155"/>
+      <c r="K8" s="155"/>
+      <c r="L8" s="155"/>
     </row>
     <row r="9" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="153"/>
-      <c r="B9" s="153"/>
-      <c r="C9" s="154" t="s">
+      <c r="A9" s="154"/>
+      <c r="B9" s="154"/>
+      <c r="C9" s="155" t="s">
         <v>178</v>
       </c>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
-      <c r="L9" s="154"/>
+      <c r="D9" s="155"/>
+      <c r="E9" s="155"/>
+      <c r="F9" s="155"/>
+      <c r="G9" s="155"/>
+      <c r="H9" s="155"/>
+      <c r="I9" s="155"/>
+      <c r="J9" s="155"/>
+      <c r="K9" s="155"/>
+      <c r="L9" s="155"/>
     </row>
     <row r="10" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="153"/>
-      <c r="B10" s="153"/>
-      <c r="C10" s="154" t="s">
+      <c r="A10" s="154"/>
+      <c r="B10" s="154"/>
+      <c r="C10" s="155" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="154"/>
-      <c r="E10" s="154"/>
-      <c r="F10" s="154"/>
-      <c r="G10" s="154"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="154"/>
-      <c r="K10" s="154"/>
-      <c r="L10" s="154"/>
+      <c r="D10" s="155"/>
+      <c r="E10" s="155"/>
+      <c r="F10" s="155"/>
+      <c r="G10" s="155"/>
+      <c r="H10" s="155"/>
+      <c r="I10" s="155"/>
+      <c r="J10" s="155"/>
+      <c r="K10" s="155"/>
+      <c r="L10" s="155"/>
     </row>
     <row r="11" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="150">
+      <c r="A11" s="156">
         <v>3</v>
       </c>
-      <c r="B11" s="151" t="s">
+      <c r="B11" s="157" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="152" t="s">
+      <c r="C11" s="158" t="s">
         <v>181</v>
       </c>
-      <c r="D11" s="152"/>
-      <c r="E11" s="152"/>
-      <c r="F11" s="152"/>
-      <c r="G11" s="152"/>
-      <c r="H11" s="152"/>
-      <c r="I11" s="152"/>
-      <c r="J11" s="152"/>
-      <c r="K11" s="152"/>
-      <c r="L11" s="152" t="s">
+      <c r="D11" s="158"/>
+      <c r="E11" s="158"/>
+      <c r="F11" s="158"/>
+      <c r="G11" s="158"/>
+      <c r="H11" s="158"/>
+      <c r="I11" s="158"/>
+      <c r="J11" s="158"/>
+      <c r="K11" s="158"/>
+      <c r="L11" s="158" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="150"/>
-      <c r="B12" s="151"/>
-      <c r="C12" s="152" t="s">
+      <c r="A12" s="156"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="158" t="s">
         <v>183</v>
       </c>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
-      <c r="F12" s="152"/>
-      <c r="G12" s="152"/>
-      <c r="H12" s="152"/>
-      <c r="I12" s="152"/>
-      <c r="J12" s="152"/>
-      <c r="K12" s="152"/>
-      <c r="L12" s="152"/>
+      <c r="D12" s="158"/>
+      <c r="E12" s="158"/>
+      <c r="F12" s="158"/>
+      <c r="G12" s="158"/>
+      <c r="H12" s="158"/>
+      <c r="I12" s="158"/>
+      <c r="J12" s="158"/>
+      <c r="K12" s="158"/>
+      <c r="L12" s="158"/>
     </row>
     <row r="13" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="150"/>
-      <c r="B13" s="151"/>
-      <c r="C13" s="152" t="s">
+      <c r="A13" s="156"/>
+      <c r="B13" s="157"/>
+      <c r="C13" s="158" t="s">
         <v>184</v>
       </c>
-      <c r="D13" s="152"/>
-      <c r="E13" s="152"/>
-      <c r="F13" s="152"/>
-      <c r="G13" s="152"/>
-      <c r="H13" s="152"/>
-      <c r="I13" s="152"/>
-      <c r="J13" s="152"/>
-      <c r="K13" s="152"/>
-      <c r="L13" s="152"/>
+      <c r="D13" s="158"/>
+      <c r="E13" s="158"/>
+      <c r="F13" s="158"/>
+      <c r="G13" s="158"/>
+      <c r="H13" s="158"/>
+      <c r="I13" s="158"/>
+      <c r="J13" s="158"/>
+      <c r="K13" s="158"/>
+      <c r="L13" s="158"/>
     </row>
     <row r="14" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="147">
+      <c r="A14" s="159">
         <v>4</v>
       </c>
-      <c r="B14" s="147" t="s">
+      <c r="B14" s="159" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="148" t="s">
+      <c r="C14" s="160" t="s">
         <v>186</v>
       </c>
-      <c r="D14" s="148"/>
-      <c r="E14" s="148"/>
-      <c r="F14" s="148"/>
-      <c r="G14" s="148"/>
-      <c r="H14" s="148"/>
-      <c r="I14" s="148"/>
-      <c r="J14" s="148"/>
-      <c r="K14" s="148"/>
-      <c r="L14" s="149" t="s">
+      <c r="D14" s="160"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="160"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
+      <c r="L14" s="161" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="147"/>
-      <c r="B15" s="147"/>
-      <c r="C15" s="148" t="s">
+      <c r="A15" s="159"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="160" t="s">
         <v>188</v>
       </c>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="148"/>
-      <c r="K15" s="148"/>
-      <c r="L15" s="149"/>
+      <c r="D15" s="160"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="160"/>
+      <c r="L15" s="161"/>
     </row>
     <row r="16" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="147"/>
-      <c r="B16" s="147"/>
-      <c r="C16" s="148" t="s">
+      <c r="A16" s="159"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="160" t="s">
         <v>189</v>
       </c>
-      <c r="D16" s="148"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="148"/>
-      <c r="K16" s="148"/>
-      <c r="L16" s="149"/>
+      <c r="D16" s="160"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
+      <c r="L16" s="161"/>
     </row>
     <row r="17" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="145">
+      <c r="A17" s="162">
         <v>5</v>
       </c>
-      <c r="B17" s="145" t="s">
+      <c r="B17" s="162" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="146" t="s">
+      <c r="C17" s="163" t="s">
         <v>191</v>
       </c>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
-      <c r="H17" s="146"/>
-      <c r="I17" s="146"/>
-      <c r="J17" s="146"/>
-      <c r="K17" s="146"/>
-      <c r="L17" s="146" t="s">
+      <c r="D17" s="163"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="163"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="163"/>
+      <c r="J17" s="163"/>
+      <c r="K17" s="163"/>
+      <c r="L17" s="163" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="145"/>
-      <c r="B18" s="145"/>
-      <c r="C18" s="146" t="s">
+      <c r="A18" s="162"/>
+      <c r="B18" s="162"/>
+      <c r="C18" s="163" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="146"/>
-      <c r="E18" s="146"/>
-      <c r="F18" s="146"/>
-      <c r="G18" s="146"/>
-      <c r="H18" s="146"/>
-      <c r="I18" s="146"/>
-      <c r="J18" s="146"/>
-      <c r="K18" s="146"/>
-      <c r="L18" s="146"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="163"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="163"/>
+      <c r="J18" s="163"/>
+      <c r="K18" s="163"/>
+      <c r="L18" s="163"/>
     </row>
     <row r="19" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="145"/>
-      <c r="B19" s="145"/>
-      <c r="C19" s="146" t="s">
+      <c r="A19" s="162"/>
+      <c r="B19" s="162"/>
+      <c r="C19" s="163" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="146"/>
-      <c r="H19" s="146"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="146"/>
-      <c r="K19" s="146"/>
-      <c r="L19" s="146"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="163"/>
+      <c r="F19" s="163"/>
+      <c r="G19" s="163"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="163"/>
+      <c r="J19" s="163"/>
+      <c r="K19" s="163"/>
+      <c r="L19" s="163"/>
     </row>
     <row r="20" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="145"/>
-      <c r="B20" s="145"/>
-      <c r="C20" s="146" t="s">
+      <c r="A20" s="162"/>
+      <c r="B20" s="162"/>
+      <c r="C20" s="163" t="s">
         <v>195</v>
       </c>
-      <c r="D20" s="146"/>
-      <c r="E20" s="146"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="146"/>
-      <c r="I20" s="146"/>
-      <c r="J20" s="146"/>
-      <c r="K20" s="146"/>
-      <c r="L20" s="146"/>
+      <c r="D20" s="163"/>
+      <c r="E20" s="163"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="163"/>
+      <c r="H20" s="163"/>
+      <c r="I20" s="163"/>
+      <c r="J20" s="163"/>
+      <c r="K20" s="163"/>
+      <c r="L20" s="163"/>
     </row>
     <row r="21" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="145"/>
-      <c r="B21" s="145"/>
-      <c r="C21" s="146" t="s">
+      <c r="A21" s="162"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="163" t="s">
         <v>196</v>
       </c>
-      <c r="D21" s="146"/>
-      <c r="E21" s="146"/>
-      <c r="F21" s="146"/>
-      <c r="G21" s="146"/>
-      <c r="H21" s="146"/>
-      <c r="I21" s="146"/>
-      <c r="J21" s="146"/>
-      <c r="K21" s="146"/>
-      <c r="L21" s="146"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="163"/>
+      <c r="F21" s="163"/>
+      <c r="G21" s="163"/>
+      <c r="H21" s="163"/>
+      <c r="I21" s="163"/>
+      <c r="J21" s="163"/>
+      <c r="K21" s="163"/>
+      <c r="L21" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="C10:K10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:K14"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="C15:K15"/>
-    <mergeCell ref="C16:K16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="C17:K17"/>
@@ -4336,6 +4310,32 @@
     <mergeCell ref="C19:K19"/>
     <mergeCell ref="C20:K20"/>
     <mergeCell ref="C21:K21"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="C10:K10"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="C6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added scripts for area-level indicators and demographics overview
</commit_message>
<xml_diff>
--- a/IRQ_2021HNO_Inter-sectoral_PIN-Severity_DRAFT-ENDORSED_AWG-IMWG_2020_09_03.xlsx
+++ b/IRQ_2021HNO_Inter-sectoral_PIN-Severity_DRAFT-ENDORSED_AWG-IMWG_2020_09_03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\OneDrive\Documents\REACH2020\MCNA VIII\MCNA20_Analysis_IRQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F244538-4739-4513-AFD7-CEAE341313B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEDFC3A-5226-40B1-BB11-6C702B505F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DE93082-DA25-4047-BA9C-ECE0BEA4BEF8}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="229">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -296,15 +296,6 @@
   </si>
   <si>
     <t>Food Consumption Score (FCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceptable </t>
-  </si>
-  <si>
-    <t>Borderline</t>
-  </si>
-  <si>
-    <t>Poor</t>
   </si>
   <si>
     <t xml:space="preserve">Household Hunger Scale </t>
@@ -411,18 +402,6 @@
     <t xml:space="preserve">% of locations in which HHs are reportedly concerned about explosive devices (mines, UXOs, IEDs) 
 and 
 % locations where [ERW, landmine, UXO] was reported in last three months </t>
-  </si>
-  <si>
-    <t>HHs are not concerned about explosive devices (mines, UXOs, IEDs) AND location did not report incidents related to IEDs and/or UXOs in the last 3 months</t>
-  </si>
-  <si>
-    <t>HHs are somewhat concerned about explosive devices (mines, UXOs, IEDs) AND location did not report incidents related to IEDs and/or UXOs in the last 3 months</t>
-  </si>
-  <si>
-    <t>HHs are very concerned about explosive devices (mines, UXOs, IEDs) AND location did not report incidents related to IEDs and/or UXOs in the last 3 months</t>
-  </si>
-  <si>
-    <t>HHs are very concerned about explosive devices (mines, UXOs, IEDs) AND location reported incidents related to IEDs and/or UXOs in the last 3 months</t>
   </si>
   <si>
     <t xml:space="preserve">Protection - HLP </t>
@@ -794,6 +773,35 @@
   </si>
   <si>
     <t>S20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceptable consumption &gt;=42.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceptable consumption, but deteriorating  &gt;=42.5 
++ HHS &gt; 0 </t>
+  </si>
+  <si>
+    <t>Borderline consumption 28.5- 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor consumption =&lt;28 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor consumption 
++ HHS 5-6 </t>
+  </si>
+  <si>
+    <t>No locations are reporting that HHs are concerned with explosive devices and no locations have reported incidents related to explosive devices.</t>
+  </si>
+  <si>
+    <t>Less than 10% of locations are reporting that HHs are somewhat/very concerned with explosive devices and less than 5% of locations have reported incidents related to explosive devices.</t>
+  </si>
+  <si>
+    <t>Between 10% and 30% of locations are reporting that HHs are somewhat/very concerned with explosive devices and more than 5% of locations have reported incidents related to explosive devices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than 30% of locations are reporting that HHs are somewhat concerned with explosive devices. </t>
   </si>
 </sst>
 </file>
@@ -2273,6 +2281,36 @@
     <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2280,36 +2318,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2370,7 +2378,7 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
+      <sheetData sheetId="16" refreshError="1"/>
       <sheetData sheetId="17"/>
     </sheetDataSet>
   </externalBook>
@@ -2417,7 +2425,7 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
+      <sheetData sheetId="16" refreshError="1"/>
       <sheetData sheetId="17"/>
     </sheetDataSet>
   </externalBook>
@@ -2770,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2565E548-5449-442A-A965-6E689A09088F}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="83" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="83" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2788,7 +2796,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="139" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B1" s="139"/>
       <c r="C1" s="139"/>
@@ -2809,7 +2817,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="140" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2882,7 +2890,7 @@
       <c r="M5" s="82"/>
       <c r="N5" s="75"/>
       <c r="O5" s="79" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="78" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2905,7 +2913,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="141" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>10</v>
@@ -2927,7 +2935,7 @@
       </c>
       <c r="N6" s="18"/>
       <c r="O6" s="80" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="37.5" x14ac:dyDescent="0.35">
@@ -2950,27 +2958,27 @@
         <v>20</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="88" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J7" s="89" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K7" s="90" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L7" s="91" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="M7" s="92" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="N7" s="24"/>
       <c r="O7" s="32" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.35">
@@ -2990,10 +2998,10 @@
         <v>24</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="H8" s="30" t="s">
         <v>25</v>
@@ -3081,7 +3089,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="98" t="s">
@@ -3124,7 +3132,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H11" s="39"/>
       <c r="I11" s="98" t="s">
@@ -3167,7 +3175,7 @@
         <v>34</v>
       </c>
       <c r="G12" s="143" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="H12" s="144"/>
       <c r="I12" s="98" t="s">
@@ -3210,7 +3218,7 @@
         <v>34</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H13" s="39"/>
       <c r="I13" s="98" t="s">
@@ -3253,25 +3261,25 @@
         <v>34</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>25</v>
       </c>
       <c r="I14" s="98" t="s">
-        <v>71</v>
+        <v>220</v>
       </c>
       <c r="J14" s="99" t="s">
-        <v>50</v>
+        <v>221</v>
       </c>
       <c r="K14" s="100" t="s">
-        <v>72</v>
+        <v>222</v>
       </c>
       <c r="L14" s="101" t="s">
-        <v>73</v>
+        <v>223</v>
       </c>
       <c r="M14" s="102" t="s">
-        <v>50</v>
+        <v>224</v>
       </c>
       <c r="N14" s="45"/>
       <c r="O14" s="32" t="s">
@@ -3292,33 +3300,33 @@
         <v>23</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H15" s="39"/>
       <c r="I15" s="103" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="104" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="105" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="104" t="s">
+      <c r="M15" s="107" t="s">
         <v>76</v>
-      </c>
-      <c r="K15" s="105" t="s">
-        <v>77</v>
-      </c>
-      <c r="L15" s="106" t="s">
-        <v>78</v>
-      </c>
-      <c r="M15" s="107" t="s">
-        <v>79</v>
       </c>
       <c r="N15" s="47"/>
       <c r="O15" s="32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="26" x14ac:dyDescent="0.35">
@@ -3326,7 +3334,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C16" s="48" t="s">
         <v>17</v>
@@ -3335,33 +3343,33 @@
         <v>18</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F16" s="48" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="48" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H16" s="48"/>
       <c r="I16" s="108" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="109" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="111" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="109" t="s">
+      <c r="M16" s="112" t="s">
         <v>84</v>
-      </c>
-      <c r="K16" s="110" t="s">
-        <v>85</v>
-      </c>
-      <c r="L16" s="111" t="s">
-        <v>86</v>
-      </c>
-      <c r="M16" s="112" t="s">
-        <v>87</v>
       </c>
       <c r="N16" s="51"/>
       <c r="O16" s="32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="40" x14ac:dyDescent="0.35">
@@ -3369,7 +3377,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C17" s="48" t="s">
         <v>17</v>
@@ -3378,29 +3386,29 @@
         <v>23</v>
       </c>
       <c r="E17" s="53" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F17" s="48" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H17" s="48"/>
       <c r="I17" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" s="109" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17" s="110" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="111" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="109" t="s">
+      <c r="M17" s="112" t="s">
         <v>90</v>
-      </c>
-      <c r="K17" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="L17" s="111" t="s">
-        <v>92</v>
-      </c>
-      <c r="M17" s="112" t="s">
-        <v>93</v>
       </c>
       <c r="N17" s="54"/>
       <c r="O17" s="32" t="s">
@@ -3412,7 +3420,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C18" s="48" t="s">
         <v>63</v>
@@ -3421,26 +3429,26 @@
         <v>23</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F18" s="48" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H18" s="50"/>
       <c r="I18" s="108" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J18" s="109" t="s">
         <v>50</v>
       </c>
       <c r="K18" s="110" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L18" s="111" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M18" s="112" t="s">
         <v>50</v>
@@ -3455,7 +3463,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19" s="55" t="s">
         <v>63</v>
@@ -3464,41 +3472,41 @@
         <v>18</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F19" s="55" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="55" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H19" s="57"/>
       <c r="I19" s="113" t="s">
+        <v>98</v>
+      </c>
+      <c r="J19" s="114" t="s">
+        <v>99</v>
+      </c>
+      <c r="K19" s="115" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" s="116" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="114" t="s">
+      <c r="M19" s="117" t="s">
         <v>102</v>
-      </c>
-      <c r="K19" s="115" t="s">
-        <v>103</v>
-      </c>
-      <c r="L19" s="116" t="s">
-        <v>104</v>
-      </c>
-      <c r="M19" s="117" t="s">
-        <v>105</v>
       </c>
       <c r="N19" s="58"/>
       <c r="O19" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="70" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="80" x14ac:dyDescent="0.35">
       <c r="A20" s="26">
         <v>14</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C20" s="37" t="s">
         <v>17</v>
@@ -3507,7 +3515,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F20" s="37" t="s">
         <v>34</v>
@@ -3517,21 +3525,21 @@
       </c>
       <c r="H20" s="39"/>
       <c r="I20" s="113" t="s">
-        <v>108</v>
+        <v>225</v>
       </c>
       <c r="J20" s="114" t="s">
-        <v>109</v>
+        <v>226</v>
       </c>
       <c r="K20" s="115" t="s">
-        <v>110</v>
+        <v>227</v>
       </c>
       <c r="L20" s="116" t="s">
-        <v>111</v>
+        <v>228</v>
       </c>
       <c r="M20" s="117"/>
       <c r="N20" s="24"/>
       <c r="O20" s="25" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="120" x14ac:dyDescent="0.35">
@@ -3539,7 +3547,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>17</v>
@@ -3548,26 +3556,26 @@
         <v>18</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>34</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H21" s="39"/>
       <c r="I21" s="118" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="J21" s="119" t="s">
         <v>50</v>
       </c>
       <c r="K21" s="120" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="L21" s="121" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="M21" s="122" t="s">
         <v>50</v>
@@ -3582,7 +3590,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C22" s="61" t="s">
         <v>63</v>
@@ -3591,29 +3599,29 @@
         <v>23</v>
       </c>
       <c r="E22" s="145" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F22" s="146" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="146" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="H22" s="39"/>
       <c r="I22" s="103" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J22" s="104" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K22" s="105" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="L22" s="106" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="M22" s="107" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="N22" s="47"/>
       <c r="O22" s="32" t="s">
@@ -3625,38 +3633,38 @@
         <v>17</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D23" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F23" s="37" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="H23" s="39"/>
       <c r="I23" s="98" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="J23" s="99" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="K23" s="100" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="L23" s="101" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="M23" s="102" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="N23" s="24"/>
       <c r="O23" s="32" t="s">
@@ -3668,7 +3676,7 @@
         <v>18</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>17</v>
@@ -3677,33 +3685,33 @@
         <v>18</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G24" s="37" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="39"/>
       <c r="I24" s="98" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="J24" s="99" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="K24" s="100" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="L24" s="101" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="M24" s="102" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="N24" s="24"/>
       <c r="O24" s="32" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="90" x14ac:dyDescent="0.35">
@@ -3711,38 +3719,38 @@
         <v>19</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D25" s="61" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F25" s="37" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H25" s="39"/>
       <c r="I25" s="123" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J25" s="124" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K25" s="125" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="L25" s="121" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="M25" s="122" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="N25" s="24"/>
       <c r="O25" s="32" t="s">
@@ -3754,40 +3762,40 @@
         <v>20</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D26" s="61" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F26" s="37" t="s">
         <v>34</v>
       </c>
       <c r="G26" s="142" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H26" s="62" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="123" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="J26" s="124" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="K26" s="125" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="L26" s="121" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="M26" s="122" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="N26" s="24"/>
       <c r="O26" s="32" t="s">
@@ -3799,7 +3807,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C27" s="40" t="s">
         <v>17</v>
@@ -3808,29 +3816,29 @@
         <v>23</v>
       </c>
       <c r="E27" s="60" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F27" s="40" t="s">
         <v>34</v>
       </c>
       <c r="G27" s="40" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H27" s="64"/>
       <c r="I27" s="118" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="J27" s="126" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="K27" s="127" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="L27" s="128" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="M27" s="129" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="N27" s="65"/>
       <c r="O27" s="32" t="s">
@@ -3842,7 +3850,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C28" s="68" t="s">
         <v>17</v>
@@ -3851,25 +3859,25 @@
         <v>23</v>
       </c>
       <c r="E28" s="70" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F28" s="68" t="s">
         <v>34</v>
       </c>
       <c r="G28" s="68" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H28" s="71"/>
       <c r="I28" s="130" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="J28" s="131"/>
       <c r="K28" s="132" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L28" s="133"/>
       <c r="M28" s="134" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="N28" s="65"/>
       <c r="O28" s="32" t="s">
@@ -3932,7 +3940,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="137" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B1" s="137"/>
       <c r="C1" s="136"/>
@@ -3962,159 +3970,159 @@
     </row>
     <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="138" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="138" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="161" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
+      <c r="L3" s="138" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="162">
+        <v>1</v>
+      </c>
+      <c r="B4" s="162" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="163" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
+      <c r="K4" s="163"/>
+      <c r="L4" s="163" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="162"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="163" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="138" t="s">
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+    </row>
+    <row r="6" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="162"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
+      <c r="K6" s="163"/>
+      <c r="L6" s="163"/>
+    </row>
+    <row r="7" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="159">
+        <v>2</v>
+      </c>
+      <c r="B7" s="159" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="151"/>
-      <c r="K3" s="151"/>
-      <c r="L3" s="138" t="s">
+      <c r="C7" s="160" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="152">
-        <v>1</v>
-      </c>
-      <c r="B4" s="152" t="s">
+      <c r="D7" s="160"/>
+      <c r="E7" s="160"/>
+      <c r="F7" s="160"/>
+      <c r="G7" s="160"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
+      <c r="K7" s="160"/>
+      <c r="L7" s="160" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="153" t="s">
+    </row>
+    <row r="8" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="159"/>
+      <c r="B8" s="159"/>
+      <c r="C8" s="160" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="153" t="s">
+      <c r="D8" s="160"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="160"/>
+      <c r="K8" s="160"/>
+      <c r="L8" s="160"/>
+    </row>
+    <row r="9" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="159"/>
+      <c r="B9" s="159"/>
+      <c r="C9" s="160" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="152"/>
-      <c r="B5" s="152"/>
-      <c r="C5" s="153" t="s">
+      <c r="D9" s="160"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="160"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="160"/>
+      <c r="K9" s="160"/>
+      <c r="L9" s="160"/>
+    </row>
+    <row r="10" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="159"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="160" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="153"/>
-      <c r="E5" s="153"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
-      <c r="K5" s="153"/>
-      <c r="L5" s="153"/>
-    </row>
-    <row r="6" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="152"/>
-      <c r="B6" s="152"/>
-      <c r="C6" s="153" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="153"/>
-      <c r="E6" s="153"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="153"/>
-    </row>
-    <row r="7" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="154">
-        <v>2</v>
-      </c>
-      <c r="B7" s="154" t="s">
-        <v>174</v>
-      </c>
-      <c r="C7" s="155" t="s">
-        <v>175</v>
-      </c>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="155"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="155"/>
-      <c r="J7" s="155"/>
-      <c r="K7" s="155"/>
-      <c r="L7" s="155" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="154"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="155" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" s="155"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="155"/>
-      <c r="H8" s="155"/>
-      <c r="I8" s="155"/>
-      <c r="J8" s="155"/>
-      <c r="K8" s="155"/>
-      <c r="L8" s="155"/>
-    </row>
-    <row r="9" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="154"/>
-      <c r="B9" s="154"/>
-      <c r="C9" s="155" t="s">
-        <v>178</v>
-      </c>
-      <c r="D9" s="155"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="155"/>
-      <c r="H9" s="155"/>
-      <c r="I9" s="155"/>
-      <c r="J9" s="155"/>
-      <c r="K9" s="155"/>
-      <c r="L9" s="155"/>
-    </row>
-    <row r="10" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="154"/>
-      <c r="B10" s="154"/>
-      <c r="C10" s="155" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="155"/>
-      <c r="E10" s="155"/>
-      <c r="F10" s="155"/>
-      <c r="G10" s="155"/>
-      <c r="H10" s="155"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="155"/>
-      <c r="K10" s="155"/>
-      <c r="L10" s="155"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="160"/>
+      <c r="F10" s="160"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="160"/>
+      <c r="K10" s="160"/>
+      <c r="L10" s="160"/>
     </row>
     <row r="11" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="156">
         <v>3</v>
       </c>
       <c r="B11" s="157" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C11" s="158" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D11" s="158"/>
       <c r="E11" s="158"/>
@@ -4125,14 +4133,14 @@
       <c r="J11" s="158"/>
       <c r="K11" s="158"/>
       <c r="L11" s="158" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="156"/>
       <c r="B12" s="157"/>
       <c r="C12" s="158" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D12" s="158"/>
       <c r="E12" s="158"/>
@@ -4148,7 +4156,7 @@
       <c r="A13" s="156"/>
       <c r="B13" s="157"/>
       <c r="C13" s="158" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D13" s="158"/>
       <c r="E13" s="158"/>
@@ -4161,147 +4169,173 @@
       <c r="L13" s="158"/>
     </row>
     <row r="14" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="159">
+      <c r="A14" s="153">
         <v>4</v>
       </c>
-      <c r="B14" s="159" t="s">
+      <c r="B14" s="153" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="154" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="154"/>
+      <c r="E14" s="154"/>
+      <c r="F14" s="154"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="154"/>
+      <c r="L14" s="155" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="153"/>
+      <c r="B15" s="153"/>
+      <c r="C15" s="154" t="s">
+        <v>181</v>
+      </c>
+      <c r="D15" s="154"/>
+      <c r="E15" s="154"/>
+      <c r="F15" s="154"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="154"/>
+      <c r="K15" s="154"/>
+      <c r="L15" s="155"/>
+    </row>
+    <row r="16" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="153"/>
+      <c r="B16" s="153"/>
+      <c r="C16" s="154" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="155"/>
+    </row>
+    <row r="17" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="151">
+        <v>5</v>
+      </c>
+      <c r="B17" s="151" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="152" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="152"/>
+      <c r="E17" s="152"/>
+      <c r="F17" s="152"/>
+      <c r="G17" s="152"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="152"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="152"/>
+      <c r="L17" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="160" t="s">
+    </row>
+    <row r="18" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="151"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="152" t="s">
         <v>186</v>
       </c>
-      <c r="D14" s="160"/>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
-      <c r="L14" s="161" t="s">
+      <c r="D18" s="152"/>
+      <c r="E18" s="152"/>
+      <c r="F18" s="152"/>
+      <c r="G18" s="152"/>
+      <c r="H18" s="152"/>
+      <c r="I18" s="152"/>
+      <c r="J18" s="152"/>
+      <c r="K18" s="152"/>
+      <c r="L18" s="152"/>
+    </row>
+    <row r="19" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="151"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="152" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="159"/>
-      <c r="B15" s="159"/>
-      <c r="C15" s="160" t="s">
+      <c r="D19" s="152"/>
+      <c r="E19" s="152"/>
+      <c r="F19" s="152"/>
+      <c r="G19" s="152"/>
+      <c r="H19" s="152"/>
+      <c r="I19" s="152"/>
+      <c r="J19" s="152"/>
+      <c r="K19" s="152"/>
+      <c r="L19" s="152"/>
+    </row>
+    <row r="20" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="151"/>
+      <c r="B20" s="151"/>
+      <c r="C20" s="152" t="s">
         <v>188</v>
       </c>
-      <c r="D15" s="160"/>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
-      <c r="L15" s="161"/>
-    </row>
-    <row r="16" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="159"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="160" t="s">
+      <c r="D20" s="152"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="152"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="152"/>
+      <c r="J20" s="152"/>
+      <c r="K20" s="152"/>
+      <c r="L20" s="152"/>
+    </row>
+    <row r="21" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="151"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="152" t="s">
         <v>189</v>
       </c>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
-      <c r="L16" s="161"/>
-    </row>
-    <row r="17" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="162">
-        <v>5</v>
-      </c>
-      <c r="B17" s="162" t="s">
-        <v>190</v>
-      </c>
-      <c r="C17" s="163" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" s="163"/>
-      <c r="E17" s="163"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="163"/>
-      <c r="H17" s="163"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="163"/>
-      <c r="K17" s="163"/>
-      <c r="L17" s="163" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="162"/>
-      <c r="B18" s="162"/>
-      <c r="C18" s="163" t="s">
-        <v>193</v>
-      </c>
-      <c r="D18" s="163"/>
-      <c r="E18" s="163"/>
-      <c r="F18" s="163"/>
-      <c r="G18" s="163"/>
-      <c r="H18" s="163"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="163"/>
-      <c r="K18" s="163"/>
-      <c r="L18" s="163"/>
-    </row>
-    <row r="19" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="162"/>
-      <c r="B19" s="162"/>
-      <c r="C19" s="163" t="s">
-        <v>194</v>
-      </c>
-      <c r="D19" s="163"/>
-      <c r="E19" s="163"/>
-      <c r="F19" s="163"/>
-      <c r="G19" s="163"/>
-      <c r="H19" s="163"/>
-      <c r="I19" s="163"/>
-      <c r="J19" s="163"/>
-      <c r="K19" s="163"/>
-      <c r="L19" s="163"/>
-    </row>
-    <row r="20" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="162"/>
-      <c r="B20" s="162"/>
-      <c r="C20" s="163" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" s="163"/>
-      <c r="E20" s="163"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="163"/>
-      <c r="H20" s="163"/>
-      <c r="I20" s="163"/>
-      <c r="J20" s="163"/>
-      <c r="K20" s="163"/>
-      <c r="L20" s="163"/>
-    </row>
-    <row r="21" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="162"/>
-      <c r="B21" s="162"/>
-      <c r="C21" s="163" t="s">
-        <v>196</v>
-      </c>
-      <c r="D21" s="163"/>
-      <c r="E21" s="163"/>
-      <c r="F21" s="163"/>
-      <c r="G21" s="163"/>
-      <c r="H21" s="163"/>
-      <c r="I21" s="163"/>
-      <c r="J21" s="163"/>
-      <c r="K21" s="163"/>
-      <c r="L21" s="163"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="152"/>
+      <c r="J21" s="152"/>
+      <c r="K21" s="152"/>
+      <c r="L21" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="C10:K10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C16:K16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="C17:K17"/>
@@ -4310,32 +4344,6 @@
     <mergeCell ref="C19:K19"/>
     <mergeCell ref="C20:K20"/>
     <mergeCell ref="C21:K21"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:K14"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="C15:K15"/>
-    <mergeCell ref="C16:K16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="C10:K10"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="C6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>